<commit_message>
change module nilai add kelas
</commit_message>
<xml_diff>
--- a/upload/format_mapel.xlsx
+++ b/upload/format_mapel.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROBBY\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\silusi\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CB134F-EF3F-4783-BBBC-C4559659715F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0E717172-3C02-4D07-A468-817235BFE0E7}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>mapel</t>
   </si>
@@ -36,9 +35,6 @@
     <t>Bahasa Indonesia</t>
   </si>
   <si>
-    <t>Matematika</t>
-  </si>
-  <si>
     <t>Bahasa Inggris</t>
   </si>
   <si>
@@ -58,12 +54,45 @@
   </si>
   <si>
     <t>Geografi</t>
+  </si>
+  <si>
+    <t>PAI</t>
+  </si>
+  <si>
+    <t>PPKN</t>
+  </si>
+  <si>
+    <t>Matematika Wajib</t>
+  </si>
+  <si>
+    <t>Seni Budaya</t>
+  </si>
+  <si>
+    <t>Penjasorkes</t>
+  </si>
+  <si>
+    <t>Prakarya</t>
+  </si>
+  <si>
+    <t>Bahasa Daerah</t>
+  </si>
+  <si>
+    <t>Sejarah Peminatan</t>
+  </si>
+  <si>
+    <t>Matematika Peminatan</t>
+  </si>
+  <si>
+    <t>Sastra Inggris</t>
+  </si>
+  <si>
+    <t>Sejarah Indonesia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,16 +437,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B4EF20-18D4-4820-8FEB-F5440C998BE4}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -425,76 +454,156 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>